<commit_message>
implemented controller evaluation index method +
</commit_message>
<xml_diff>
--- a/WSafe/WSafe.Web/SG-SST/1. PLANEAR/2022/1.1.6/FRSST-008 Formato Acta de reunion del copasst(1).xlsx
+++ b/WSafe/WSafe.Web/SG-SST/1. PLANEAR/2022/1.1.6/FRSST-008 Formato Acta de reunion del copasst(1).xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Hewlett Packard\Desktop\SG-SST Sergio Escobar\1. Planear\1.1.6 COPASST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\WSafe\WSafe.Web\SG-SST\1. PLANEAR\2022\1.1.6\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361B9375-5F48-4468-952C-458670D4DD19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="7155" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACTA DE REUNION" sheetId="1" r:id="rId1"/>
     <sheet name="PLAN DE ACCIÓN " sheetId="3" r:id="rId2"/>
     <sheet name="Control de cambios" sheetId="2" r:id="rId3"/>
+    <sheet name="ACTA DICIEMBRE-2022" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'ACTA DE REUNION'!$A$1:$F$24</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'ACTA DICIEMBRE-2022'!$A$1:$F$24</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t>HORA DE INICIO</t>
   </si>
@@ -89,15 +92,6 @@
     <t>OBJETIVO(S) DE LA REUNION (Orden del dia)</t>
   </si>
   <si>
-    <t>1.</t>
-  </si>
-  <si>
-    <t>2.</t>
-  </si>
-  <si>
-    <t>3.</t>
-  </si>
-  <si>
     <t>4.</t>
   </si>
   <si>
@@ -138,12 +132,27 @@
   </si>
   <si>
     <t>Fecha: 10/09/2018</t>
+  </si>
+  <si>
+    <t>hhhhh</t>
+  </si>
+  <si>
+    <t>Fecha: 16/12/2022</t>
+  </si>
+  <si>
+    <t>1. Verificación del acta anterior</t>
+  </si>
+  <si>
+    <t>2. Rezvisar asistencia participantes</t>
+  </si>
+  <si>
+    <t>3. Tareas a desarrollar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -421,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -475,6 +484,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -508,83 +595,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -895,14 +907,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+      <selection activeCell="A12" sqref="A12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -918,67 +930,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39"/>
-      <c r="B1" s="40"/>
-      <c r="C1" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="23" t="s">
+      <c r="A1" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="49"/>
+    </row>
+    <row r="2" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="23"/>
-    </row>
-    <row r="2" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="23"/>
+      <c r="G2" s="49"/>
     </row>
     <row r="3" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="24"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="50"/>
     </row>
     <row r="4" spans="1:7" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="36"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="31"/>
     </row>
     <row r="5" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="57"/>
+      <c r="A5" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="48"/>
     </row>
     <row r="6" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="58" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="49" t="s">
+      <c r="A6" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="49"/>
+      <c r="D6" s="29"/>
       <c r="E6" s="18" t="s">
         <v>0</v>
       </c>
@@ -987,89 +1001,89 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="36"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="31"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="26"/>
+    </row>
+    <row r="10" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="26"/>
+    </row>
+    <row r="11" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26"/>
+    </row>
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="52"/>
-    </row>
-    <row r="10" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="50" t="s">
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="26"/>
+    </row>
+    <row r="13" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="52"/>
-    </row>
-    <row r="11" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="52"/>
-    </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="50" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="52"/>
-    </row>
-    <row r="13" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="50" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="52"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="26"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
     </row>
     <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="47"/>
-      <c r="C15" s="48"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="43"/>
       <c r="D15" s="20" t="s">
         <v>5</v>
       </c>
@@ -1081,78 +1095,78 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="45"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="40"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="45"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="40"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="45"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="40"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
-      <c r="B20" s="44"/>
-      <c r="C20" s="45"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="40"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
+      <c r="A22" s="33"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
     </row>
     <row r="23" spans="1:6" ht="167.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="38"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
+      <c r="A23" s="33"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
     </row>
     <row r="24" spans="1:6" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
     </row>
     <row r="25" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
@@ -1188,12 +1202,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C1:E3"/>
+    <mergeCell ref="A4:F4"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="A22:F24"/>
     <mergeCell ref="A1:B3"/>
@@ -1210,19 +1223,20 @@
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="A13:F13"/>
     <mergeCell ref="A10:F10"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C1:E3"/>
-    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="94" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="96" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -1240,35 +1254,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="62"/>
+      <c r="A1" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="63"/>
       <c r="F1" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="65"/>
+      <c r="A2" s="64"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="66"/>
       <c r="F2" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="66"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="68"/>
+      <c r="A3" s="67"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1285,7 +1299,7 @@
         <v>17</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>16</v>
@@ -1357,10 +1371,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1372,19 +1386,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>10</v>
@@ -1399,10 +1413,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1435,4 +1449,333 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FECE676-F574-4ABA-9B4F-41AF581946EB}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="18" style="4" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="0.140625" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="49"/>
+    </row>
+    <row r="2" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="49"/>
+    </row>
+    <row r="3" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="50"/>
+    </row>
+    <row r="4" spans="1:7" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="31"/>
+    </row>
+    <row r="5" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="48"/>
+    </row>
+    <row r="6" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="29"/>
+      <c r="E6" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+    </row>
+    <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="26"/>
+    </row>
+    <row r="10" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="26"/>
+    </row>
+    <row r="11" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26"/>
+    </row>
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="26"/>
+    </row>
+    <row r="13" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="26"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+    </row>
+    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="42"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="38"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="38"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="38"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="33"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+    </row>
+    <row r="23" spans="1:6" ht="167.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="33"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+    </row>
+    <row r="24" spans="1:6" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+    </row>
+    <row r="25" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="27">
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="C1:E3"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A22:F24"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="96" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>